<commit_message>
Rerunning Stanza + results
</commit_message>
<xml_diff>
--- a/data/results/stanza_lemmas.xlsx
+++ b/data/results/stanza_lemmas.xlsx
@@ -13446,7 +13446,7 @@
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>chyrowska</t>
+          <t>chyrowski</t>
         </is>
       </c>
       <c r="E521" t="inlineStr">
@@ -20371,7 +20371,7 @@
       </c>
       <c r="D798" t="inlineStr">
         <is>
-          <t>Stanisława</t>
+          <t>Stanisław</t>
         </is>
       </c>
       <c r="E798" t="inlineStr">
@@ -20421,7 +20421,7 @@
       </c>
       <c r="D800" t="inlineStr">
         <is>
-          <t>Augusta</t>
+          <t>August</t>
         </is>
       </c>
       <c r="E800" t="inlineStr">
@@ -32821,7 +32821,7 @@
       </c>
       <c r="D1296" t="inlineStr">
         <is>
-          <t>sachsen</t>
+          <t>Sachsen</t>
         </is>
       </c>
       <c r="E1296" t="inlineStr">
@@ -32846,7 +32846,7 @@
       </c>
       <c r="D1297" t="inlineStr">
         <is>
-          <t>cobary</t>
+          <t>Cobary</t>
         </is>
       </c>
       <c r="E1297" t="inlineStr">
@@ -42796,7 +42796,7 @@
       </c>
       <c r="D1695" t="inlineStr">
         <is>
-          <t>jaja</t>
+          <t>jajo</t>
         </is>
       </c>
       <c r="E1695" t="inlineStr">

</xml_diff>